<commit_message>
making some progress on the weekly report
</commit_message>
<xml_diff>
--- a/reverse_engineer_API/reports/weekly/weekly_report_20250105.xlsx
+++ b/reverse_engineer_API/reports/weekly/weekly_report_20250105.xlsx
@@ -32,12 +32,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCCCCC"/>
+        <bgColor rgb="00CCCCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,9 +58,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -743,7 +750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -754,14 +761,34 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>OSP Production Master - Weekly Status Report</t>
+          <t>OSP Productivity</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Generated: 2025-01-05 08:00:00</t>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Completed Poles</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Last Activity</t>
         </is>
       </c>
     </row>
@@ -773,104 +800,94 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Job ID</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Utility</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Pole Count</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Utility Progress</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Utility</t>
         </is>
       </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>Current Rate</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>Previous Rate</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="inlineStr">
-        <is>
-          <t>Change</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>Total Poles</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
-        <is>
-          <t>Completed Poles</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>OSP Productivity</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Worker</t>
-        </is>
-      </c>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>Jobs Processed</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="inlineStr">
-        <is>
-          <t>Poles Completed</t>
-        </is>
-      </c>
-      <c r="D11" s="1" t="inlineStr">
-        <is>
-          <t>Avg Poles/Job</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Status Tracking</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>Job ID</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t>Pole Count</t>
-        </is>
-      </c>
-      <c r="D14" s="1" t="inlineStr">
-        <is>
-          <t>Utility</t>
-        </is>
-      </c>
-      <c r="E14" s="1" t="inlineStr">
-        <is>
-          <t>Original Status Date</t>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>Remaining</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>Completion %</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>Est. Completion Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -885,7 +902,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A8:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,123 +910,180 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Burndown Analysis</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Utility Burndown</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Utility</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Total Poles</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Completed Poles</t>
         </is>
       </c>
-      <c r="D4" s="1" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>Run Rate</t>
         </is>
       </c>
-      <c r="E4" s="1" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Est. Completion</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Unknown</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B9" t="n">
         <v>0</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C9" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.0 poles/week</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Total Poles</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Completed Poles</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Run Rate</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>Est. Completion</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.0 poles/week</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Backlog Analysis</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>Total Poles</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>Jobs</t>
         </is>
       </c>
-      <c r="D9" s="1" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr">
         <is>
           <t>Utilities</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Field</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Field Collection</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>286</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Back Office</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
         <v>0</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C19" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D19" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Back Office</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Approve for Construction</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>286</v>
+      </c>
+      <c r="C20" t="n">
         <v>4</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1024,7 +1098,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A23:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1032,47 +1106,40 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Project Schedule</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Project</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>Total Poles</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>Completed Poles</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>Progress</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>Field Users</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="F23" s="2" t="inlineStr">
         <is>
           <t>Back Office Users</t>
         </is>
       </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>Est. Completion</t>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>End Date</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added a test mode that bypasses sharepoint and arcupdate
</commit_message>
<xml_diff>
--- a/reverse_engineer_API/reports/weekly/weekly_report_20250105.xlsx
+++ b/reverse_engineer_API/reports/weekly/weekly_report_20250105.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Weekly Status" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Burndown" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Schedule" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Charts" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -58,9 +57,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -151,7 +153,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Utility Completion Rates</a:t>
+              <a:t>Utility Burndown</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -166,7 +168,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Weekly Status'!B6</f>
+              <f>'Burndown'!B24</f>
             </strRef>
           </tx>
           <spPr>
@@ -176,12 +178,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Weekly Status'!$A$7</f>
+              <f>'Burndown'!$A$25:$A$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Weekly Status'!$B$7</f>
+              <f>'Burndown'!$C$24:$B$24</f>
             </numRef>
           </val>
         </ser>
@@ -190,7 +192,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Weekly Status'!C6</f>
+              <f>'Burndown'!C24</f>
             </strRef>
           </tx>
           <spPr>
@@ -200,12 +202,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Weekly Status'!$A$7</f>
+              <f>'Burndown'!$A$25:$A$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Weekly Status'!$C$7</f>
+              <f>'Burndown'!$D$24:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -255,7 +257,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Rate</a:t>
+                  <a:t>Poles</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -288,7 +290,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>OSP Productivity</a:t>
+              <a:t>Project Burndown</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -303,7 +305,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Weekly Status'!B11</f>
+              <f>'Burndown'!B27</f>
             </strRef>
           </tx>
           <spPr>
@@ -313,12 +315,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Weekly Status'!$A$12:$A$11</f>
+              <f>'Burndown'!$A$28:$A$27</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Weekly Status'!$C$11:$B$11</f>
+              <f>'Burndown'!$C$27:$B$27</f>
             </numRef>
           </val>
         </ser>
@@ -327,7 +329,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Weekly Status'!C11</f>
+              <f>'Burndown'!C27</f>
             </strRef>
           </tx>
           <spPr>
@@ -337,12 +339,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Weekly Status'!$A$12:$A$11</f>
+              <f>'Burndown'!$A$28:$A$27</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Weekly Status'!$D$11:$C$11</f>
+              <f>'Burndown'!$D$27:$C$27</f>
             </numRef>
           </val>
         </ser>
@@ -365,7 +367,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Worker</a:t>
+                  <a:t>Project</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -392,7 +394,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Count</a:t>
+                  <a:t>Poles</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -416,7 +418,7 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>1</col>
+      <col>6</col>
       <colOff>0</colOff>
       <row>1</row>
       <rowOff>0</rowOff>
@@ -438,9 +440,9 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>9</col>
+      <col>6</col>
       <colOff>0</colOff>
-      <row>1</row>
+      <row>19</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -750,7 +752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,137 +763,263 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>OSP Productivity</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>User</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>Role</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>Completed Poles</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>Utilities</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>Last Activity</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+          <t>OSP Production Master - Weekly Status Report</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Date Range: 2024-12-29 to 2025-01-05</t>
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Utility Progress</t>
+        </is>
+      </c>
+    </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Job ID</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Utility</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Pole Count</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Utility Progress</t>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Total Poles</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Field Completed</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Back Office Completed</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Remaining Poles</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Run Rate</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>Est. Completion</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Utility</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
+          <t>Field Productivity</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Completed Poles</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>Jobs Completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Back Office Productivity</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Completed Poles</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>Jobs Completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Status Tracking</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Total Jobs</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
         <is>
           <t>Total Poles</t>
         </is>
       </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>Completed</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>Remaining</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>Completion %</t>
-        </is>
-      </c>
-      <c r="F8" s="1" t="inlineStr">
-        <is>
-          <t>Est. Completion Date</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>Change from Last Week</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>field_collection</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>43</v>
+      </c>
+      <c r="C16" t="n">
         <v>0</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>annotation</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>56</v>
+      </c>
+      <c r="C17" t="n">
         <v>0</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>sent_to_pe</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" t="n">
         <v>0</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>N/A</t>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>delivery</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>25</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>emr</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>approved</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -902,193 +1030,157 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A8:E20"/>
+  <dimension ref="A24:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>Utility</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B24" s="3" t="inlineStr">
         <is>
           <t>Total Poles</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C24" s="3" t="inlineStr">
         <is>
           <t>Completed Poles</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D24" s="3" t="inlineStr">
         <is>
           <t>Run Rate</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
+      <c r="E24" s="3" t="inlineStr">
         <is>
           <t>Est. Completion</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>Project</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>Total Poles</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>Completed Poles</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>Run Rate</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="inlineStr">
+        <is>
+          <t>Est. Completion</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Backlog Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>Total Poles</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>Jobs</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Field Collection</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>4563</v>
+      </c>
+      <c r="C32" t="n">
+        <v>97</v>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>Unknown</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0.0 poles/week</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Project</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>Total Poles</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>Completed Poles</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>Run Rate</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>Est. Completion</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Back Office</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>5027</v>
+      </c>
+      <c r="C33" t="n">
+        <v>58</v>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>Unknown</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0.0 poles/week</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Backlog Analysis</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>Total Poles</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>Jobs</t>
-        </is>
-      </c>
-      <c r="D17" s="2" t="inlineStr">
-        <is>
-          <t>Utilities</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Field Collection</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>286</v>
-      </c>
-      <c r="C18" t="n">
-        <v>4</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Back Office</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Approve for Construction</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>286</v>
-      </c>
-      <c r="C20" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1</v>
+      <c r="B34" t="n">
+        <v>12869</v>
+      </c>
+      <c r="C34" t="n">
+        <v>163</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1098,7 +1190,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A23:G23"/>
+  <dimension ref="A37:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1106,38 +1198,38 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
         <is>
           <t>Project</t>
         </is>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="B37" s="3" t="inlineStr">
         <is>
           <t>Total Poles</t>
         </is>
       </c>
-      <c r="C23" s="2" t="inlineStr">
+      <c r="C37" s="3" t="inlineStr">
         <is>
           <t>Completed Poles</t>
         </is>
       </c>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="D37" s="3" t="inlineStr">
         <is>
           <t>Progress</t>
         </is>
       </c>
-      <c r="E23" s="2" t="inlineStr">
+      <c r="E37" s="3" t="inlineStr">
         <is>
           <t>Field Users</t>
         </is>
       </c>
-      <c r="F23" s="2" t="inlineStr">
+      <c r="F37" s="3" t="inlineStr">
         <is>
           <t>Back Office Users</t>
         </is>
       </c>
-      <c r="G23" s="2" t="inlineStr">
+      <c r="G37" s="3" t="inlineStr">
         <is>
           <t>End Date</t>
         </is>
@@ -1146,23 +1238,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>